<commit_message>
export is gefixt en werkt
</commit_message>
<xml_diff>
--- a/bol_scraper/scraped_products.xlsx
+++ b/bol_scraper/scraped_products.xlsx
@@ -1,37 +1,142 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+  <si>
+    <t>Productnaam</t>
+  </si>
+  <si>
+    <t>Beschrijving</t>
+  </si>
+  <si>
+    <t>Interne referentie</t>
+  </si>
+  <si>
+    <t>EAN</t>
+  </si>
+  <si>
+    <t>Conditie</t>
+  </si>
+  <si>
+    <t>Conditie commentaar</t>
+  </si>
+  <si>
+    <t>Voorraad</t>
+  </si>
+  <si>
+    <t>Prijs</t>
+  </si>
+  <si>
+    <t>Levertijd</t>
+  </si>
+  <si>
+    <t>Afleverwijze</t>
+  </si>
+  <si>
+    <t>Te koop</t>
+  </si>
+  <si>
+    <t>Hoofdafbeelding</t>
+  </si>
+  <si>
+    <t>Marktdeelnemer</t>
+  </si>
+  <si>
+    <t>Additionele afbeeldingen</t>
+  </si>
+  <si>
+    <t>depow Mobiele Thuislader Type 2- Schuko 3,7kW -Dubbele knopaanpassing - 16A 1 fase 7 meter Kabel - 230V EV-oplader met LCD Digitaal Display - Voor Elektrische Auto's</t>
+  </si>
+  <si>
+    <t>Color Reus Waspoeder Wasmiddel - Voordeelverpakking - 90 wasbeurten - 4.5 kg</t>
+  </si>
+  <si>
+    <t>Sneller Opladen, Sneller Gaan:De elektrische autolader is 1,5 keer sneller dan de originele lader, waardoor uw oplaadtijd wordt teruggebracht tot slechts 3 tot 5 uur. Met een 16A Schuko-stekker, instelbaar tussen 6A/8A/10A/13A/16A, biedt het de flexibiliteit om aan uw behoeften te voldoen.Twee Functies, Twee Knoppen:De Type 2-kabel biedt stroominstellingen van 6A tot 16A voor gepersonaliseerd opladen met één klik. Een andere knop programmeert opladen tijdens daluren (0,5 tot 8 uur) en volgt de laadstatus in realtime via het LCD-scherm. Eenvoudige en eenvoudige bediening, helder en uitgebreid display.Direct Opladen, Overal:laad uw voertuig op waar u ook bent met toegang tot een Schuko-aansluiting. Dankzij de 7 meter lange kabel bereikt u eenvoudig uw parkeerplaats. Sluit Schuko aan, pas de instellingen aan, sluit Type 2 aan en geniet van het gemak van zorgeloos opladen zonder dat er installatie nodig is. 1,5 m van het stopcontact tot de bedieningskast. De bedieningskast kan op de vloer worden geplaatst, zodat de stekker niet los kan raken.Duurzaam en Betrouwbaar:Gemaakt van duurzaam TPU-materiaal, de lader beschikt over ingebouwde overstroom-, overspannings-, lek-, aardings-, oververhittings- en kortsluitbeveiligingen.Universele Compatibiliteit:De EV-lader type 2 is compatibel met de meeste voertuigen die zijn uitgerust met een Type 2-aansluiting, zoals Model Y/3, E-208, E-Tech, 500e, XC40/C40, EV6/Niro, Ioniq 5/Kona, EQA en andere BEV/PHEV. Onze EV-lader wordt ondersteund door een garantie van 2 jaar. Als u hulp nodig hebt, neem dan gerust contact met ons op. Wij streven ernaar u de beste oplossing te bieden.All-in-One Pakket:Het pakket bevat een 3,7 kW EV-lader, waterdichte hoes, draagriem, microvezeldoek, draagtas en stekkerhouder. De stekkerhouder bewaart handig Type 2-stekkers en kabels voor dagelijks gebruik.De comfortabele riem zorgt voor moeiteloos transport of handig ophangen aan de muur, waardoor het ideaal is voor onderweg opladen. De opvouwbare tas past in uw kofferbak, maximaliseert de ruimte en zorgt voor eenvoudig reizen. Geniet van het ultieme in EV-laadgemak en -bescherming!Wat zit er in de doos?3,7kW Mode 2 EV-lader * 1Draagriem * 1Stekkerhouder * 1Draagtas * 1Waterdichte tas * 1Microvezelstof * 1Montagebeugel * 1Hoe gebruik je EV-lader?Stap 1-Steek de stekker in de versterkte aansluitingStap 2-Stel de stroom en de vertragingstijd inStap 3-Steek de type 2 stekker in de laadpoort van de autoLet op: Alle instellingen kunnen niet worden gewizig nadat de type 2-connector in de laadpoort van het voertuig is gestoken.BasisinfoSpanning: 230VACVermogen: Max 3,68kWStroom: 6A/8A/10A/13A/16ACertificering: CE/CB/DEKRANorm: EN 62752:2024, EN 62196RCD: Type-B AC 30mA + DC 6mABedrijfstemperatuur: -25°C tot +50°CIP-classificatie: IP66 (besturingskast)IP54 (Type 2 connector)Afmetingen besturingskast: L220 xB95 xH57 (mm)Garantie: 2-jaar garantieQuestions and AnswersQ1 Il cavo di ricarica EV deve essere installato?A1 Non è necessaria alcuna installazione. È completamente plug and play. Serve solo una presa Schuko.Q2 Devo impostare la corrente ogni volta?A2 No. Il caricatore ha una funzione memoria che salva automaticamente l'ultima impostazione usata.Q3 Come posso risolvere gli errori durante l'uso?A3 Contattaci prima per assistenza. Puoi anche consultare il manuale utente per soluzioni basate sul codice errore.Q4 Come selezionare la corrente corretta?A4 Prima di impostare la corrente, verificare la corrente massima supportata dalla presa. Non superare questo limite. Si consiglia di utilizzare una presa Schuko rinforzata da 16A.</t>
+  </si>
+  <si>
+    <t>Witte Reus Waspoeder Color 4500 gr - 90 WasbeurtenColor Reusis een waspoeder vanWitte Reus, speciaal ontwikkeld vooralle gekleurde was. Deformulevan Color Reus beschermt de kleuren en zorgt ervoor dat zelanger stralen. Het poeder is nugeconcentreerder, zodat jeminder poeder nodig hebtvoor dezelfdeReuzewaskracht. De formule werkt zelfs inkoud water, wat zorgt voorenergiebesparingzonder in te boeten op waskracht. Goed voor hetmilieuen jeportemonnee!Waarom kiezen voor Witte Reus Waspoeder Color?Extra sterk tegen vlekken– Verwijdert zelfs hethardnekkigste vuiluit je kleding.Ideaal voor gezinnen–Sterke waskrachtvoor eenvoordelige prijs.Verbeterde reuzenfrisheid– Geniet van eenlanger frisse was.Effectief vanaf 20°C– Geschikt voorwastemperaturen van 20°C tot 60°C, zodat jeenergie kunt besparenzonder in te boeten op waskracht.Behoud van kleurintensiteit– Zorgt ervoor dat je gekleurde kledingstralend schoonblijft.Dosering:Gemiddelde was:Gebruik de aanbevolen hoeveelheid poeder voor een gemiddelde was.Grote was:Gebruik een hogere dosering voor grotere hoeveelheden kleding.Witte Reus– Wast een berg, kost een beetje!</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Nieuw</t>
+  </si>
+  <si>
+    <t>nvt</t>
+  </si>
+  <si>
+    <t>1-2 werkdagen</t>
+  </si>
+  <si>
+    <t>Thuisbezorgd</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>https://media.s-bol.com/goVARA82GWpG/Y6X7k9p/124x133.jpg</t>
+  </si>
+  <si>
+    <t>https://media.s-bol.com/gKKoY7nkxNrY/VRkzmM/116x155.jpg</t>
+  </si>
+  <si>
+    <t>SmartPowerDeals</t>
+  </si>
+  <si>
+    <t>https://media.s-bol.com/goVARA82GWpG/Y6X7k9p/124x133.jpg|https://media.s-bol.com/7KGEG6KN3LGy/Q1N9DXM/124x69.jpg|https://media.s-bol.com/NAgmLlMxADk2/wjE7B1g/124x124.jpg|https://media.s-bol.com/g4G5p17lLwz9/982jLXx/124x124.jpg|https://media.s-bol.com/RGmqlOnqYQVK/wjE7B1g/124x116.jpg|https://media.s-bol.com/g4OjZpEB0279/wjE7B1g/124x124.jpg|https://media.s-bol.com/m4mpOxqYzr8O/wjE7B1g/124x124.jpg|https://media.s-bol.com/NAgmLPvEVzvD/wjE7B1g/124x124.jpg|https://media.s-bol.com/m4mpOjz4pqZO/wjE7B1g/124x124.jpg|https://media.s-bol.com/7KGElx5KkR1G/1jYJXZZ/124x50.jpg|https://media.s-bol.com/q43gJ3jrl09y/1jYJXZZ/124x50.jpg</t>
+  </si>
+  <si>
+    <t>https://media.s-bol.com/gKKoY7nkxNrY/VRkzmM/116x155.jpg|https://media.s-bol.com/m6pzMPKL51LA/g3Vkgl/124x120.jpg|https://media.s-bol.com/JAgn7kLyOBky/g3Vkgl/124x124.jpg|https://media.s-bol.com/YxAJlq26ZZw0/g3Vkgl/124x124.jpg|https://media.s-bol.com/No3RKOn7BWKv/PNJgP44/124x124.jpg|https://media.s-bol.com/YxAJlZ0oJ7Rn/g3Vkgl/124x124.jpg|https://media.s-bol.com/m6pzMyOAEOPr/g3Vkgl/124x38.jpg|https://media.s-bol.com/gKKoY7nkxNrY/VRkzmM/92x123.jpg</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +151,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,130 +473,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>source_url</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>brand</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>price_text</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>price_value</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>list_price_text</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>list_price_value</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ean</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>main_image</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>all_images</t>
-        </is>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.bol.com/nl/nl/p/cozysense-hondenmand-ortopedische-hondenmand-hondenbed-60-x-42-cm-maat-s-waterdicht-hondenmanden-honden-mand-ergonomische-comfort-en-gewrichtsondersteuning-honden-bed-geschikt-als-benchkussen-wasbare-hondenmand-zwart/9300000188747632/</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CozySense® – Hondenmand – Ortopedische Hondenmand - Hondenbed - 60 X 42 Cm – Maat S - Waterdicht – Hondenmanden - Honden mand - Ergonomische Comfort en Gewrichtsondersteuning - Honden bed - Geschikt Als Benchkussen - Zwart</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CozySense</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3999,99</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>3999.99</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>49,99</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>49.99</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>8721082089562</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Ben je op zoek naar een wasbaar hondenkussen voor jouw hond? Of is jouw hond wat ouder en kan hij wel wat extra ondersteuning gebruiken? Dan is de CozySense® Orthopedische Hondenmand de perfecte keuze. Dit hondenbed geeft je trouwe viervoeter het comfort dat hij nodig heeft door een aangename slaapplek te creëren en de druk op de gewrichten te verlichten. Hierdoor geniet jouw hond van optimaal ligcomfort en worden gezondheidsproblemen voorkomen. Een onmisbaar item voor baasjes die het welzijn en comfort van hun hond vooropstellen!Voordelen van het CozySense® Ergonomische HondenmandComfort voor iedere hondWaterdichte binnenhoesVerkrijgbaar in verschillende matenAntislip onderkantStijlvol ergonomisch designComfort voor iedere hondDe hondenmand orthopedisch is gemaakt van hoogwaardig egg crate schuim. Dit schuim zorgt voor een goede drukverlichting. Hierdoor ligt de mand niet alleen comfortabel, maar is het ook perfect voor oudere honden of huisdieren met artritis. Het schuim verdeelt het gewicht gelijkmatig over de mand en vermindert de belasting op pijnlijke gewrichten. Hierdoor geniet jouw hond van een betere nachtrust en worden toekomstige gezondheidsproblemen aanzienlijk verminderd. Daarnaast bevordert de unieke structuur van het schuim de luchtstroom, waardoor je huisdier koel en comfortabel blijft, zelfs tijdens warme dagen!Waterdichte binnenhoesOnze orthopedische hondenmand is voorzien van een waterdichte binnenhoes gemaakt van hoogwaardig TPU-materiaal. Deze hoes beschermt het schuim effectief tegen morsen en ongelukjes en verlengt de levensduur van de mand aanzienlijk. De buitenhoes is gemaakt van duurzaam polyester en combineert zachtheid met weerstand tegen krassen en bijten. De buitenhoes is via de stevige rits te verwijderen en kan gewassen worden in de wasmachine.Verkrijgbaar in verschillende matenDe hondenmand is verkrijgbaar in verschillende maten (S, M, L, XL), waardoor het geschikt is voor honden van alle rassen en groottes. Of je nu een kleine hond of een grotere viervoeter hebt, er is altijd een maat die perfect past bij de behoeften van je huisdier! Het geïntegreerde handvat maakt het daarnaast eenvoudig om het bed te verplaatsen, welke maat je ook gekozen hebt.Antislip onderkantDankzij de antislip onderkant blijft het hondenbed altijd stevig op zijn plaats liggen, zelfs op gladde vloeren of tapijt. Hierdoor heeft je hond altijd een veilige plek om te rusten, zonder dat het bed verschuift. Verder zorgt de polyester composiet TPU laag voor extra bescherming tegen slijtage en vocht, wat de levensduur van het hondenbed aanzienlijk verlengt.Stijlvol ergonomisch designDe hondenmand heeft niet alleen een functioneel ontwerp, maar ook een stijlvol uiterlijk. Zo is de mand voorzien van ergonomisch verhoogde randen, die extra ondersteuning bieden aan het hoofd en de nek van je hond. Dit maakt de mand ideaal voor honden die graag tegen iets aanleunen of hun hoofd willen laten rusten tijdens het slapen. Het moderne, strakke ontwerp past daarnaast perfect in elk interieur en zorgt ervoor dat je de hondenmand ook kunt gebruiken als benchkussen of hondenbed.Bestel vandaag nog jouw CozySense® Hondenmand en geef je hond het comfort dat hij verdient!Inhoud pakket1 x CozySense® Hondenmand1 x Hoes HondenmandSpecificatiesAfmetingen: 60 x 42 x 7 cmKleur: Zwart en witMateriaal: Egg crate schuim, polyester</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>https://media.s-bol.com/RmG3DA2ApkWE/n5WYLK7/124x124.jpg</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://media.s-bol.com/RmG3DA2ApkWE/n5WYLK7/124x124.jpg|https://media.s-bol.com/JM5rBKQrAJ7g/qxWNA93/124x124.jpg|https://media.s-bol.com/3gDLP8BNBPEM/n5WYLK7/124x124.jpg|https://media.s-bol.com/BA4jqX6jpKXW/qxWNA93/124x124.jpg|https://media.s-bol.com/8nLQ0ZP51J4m/n5WYLK7/124x124.jpg|https://media.s-bol.com/4j0MPZE7QX5x/n5WYLK7/124x124.jpg|https://media.s-bol.com/7mKP2ZN51G4j/n5WYLK7/124x124.jpg|https://media.s-bol.com/YwP3NLoLzlOK/n5WYLK7/124x124.jpg|https://media.s-bol.com/VqM3KGgGwo1X/n5WYLK7/124x124.jpg|https://media.s-bol.com/ZxQ7NMqMAmPJ/n5WYLK7/124x124.jpg</t>
-        </is>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>6975828002458</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>69</v>
+      </c>
+      <c r="H2">
+        <v>149.95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>5410091757106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>25.19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>5410091757106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>69</v>
+      </c>
+      <c r="H4">
+        <v>25.19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="N3" r:id="rId4"/>
+    <hyperlink ref="L4" r:id="rId5"/>
+    <hyperlink ref="N4" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>